<commit_message>
update notes and trial_info spreadsheet to include crude look of where the beamwidth change came from
</commit_message>
<xml_diff>
--- a/trial_info.xlsx
+++ b/trial_info.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MURI_4TB/grampus/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wu-jung/code_git/grampus_clicks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C80DB01-E58A-D54B-9035-E3D7839C8CF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBA358C-96E5-C248-B050-D8206F4F5D54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" xr2:uid="{1C0AAE96-BBD7-814F-AEB4-40BBBA93F1E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>am</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>video_underwater_frame_dolphin_turn</t>
+  </si>
+  <si>
+    <t>video_underwater_frame_catch</t>
+  </si>
+  <si>
+    <t>video_underwater_frame_all_cups_in_water</t>
   </si>
 </sst>
 </file>
@@ -469,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF83CBD-1E45-4F47-9FF6-91707150864B}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,12 +490,12 @@
     <col min="8" max="8" width="26" customWidth="1"/>
     <col min="9" max="9" width="28" customWidth="1"/>
     <col min="10" max="10" width="29.83203125" customWidth="1"/>
-    <col min="11" max="11" width="35" customWidth="1"/>
-    <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="13" max="13" width="29.83203125" customWidth="1"/>
+    <col min="11" max="13" width="35" customWidth="1"/>
+    <col min="14" max="14" width="26" customWidth="1"/>
+    <col min="15" max="15" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -524,13 +530,19 @@
         <v>27</v>
       </c>
       <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20150426</v>
       </c>
@@ -564,8 +576,11 @@
       <c r="K2">
         <v>9197</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>9376</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20150426</v>
       </c>
@@ -600,7 +615,7 @@
         <v>11668</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20150426</v>
       </c>
@@ -635,7 +650,7 @@
         <v>13881</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20150426</v>
       </c>
@@ -669,14 +684,14 @@
       <c r="K5">
         <v>15371</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>24</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>2395</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20150426</v>
       </c>
@@ -710,14 +725,14 @@
       <c r="K6">
         <v>16748</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>24</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>3450</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20150427</v>
       </c>
@@ -749,16 +764,22 @@
         <v>7464</v>
       </c>
       <c r="K7">
-        <v>7813</v>
-      </c>
-      <c r="L7" t="s">
+        <v>7883</v>
+      </c>
+      <c r="L7">
+        <v>7987</v>
+      </c>
+      <c r="M7">
+        <v>8097</v>
+      </c>
+      <c r="N7" t="s">
         <v>26</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>6545</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20150427</v>
       </c>
@@ -792,14 +813,17 @@
       <c r="K8">
         <v>9795</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8">
+        <v>9909</v>
+      </c>
+      <c r="N8" t="s">
         <v>26</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>8860</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20150427</v>
       </c>
@@ -833,14 +857,17 @@
       <c r="K9">
         <v>11271</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9">
+        <v>11458</v>
+      </c>
+      <c r="N9" t="s">
         <v>26</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>10215</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20150427</v>
       </c>
@@ -874,11 +901,62 @@
       <c r="K10">
         <v>14308</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10">
+        <v>14445</v>
+      </c>
+      <c r="N10" t="s">
         <v>26</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>13255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <f>J7/29.97</f>
+        <v>249.04904904904905</v>
+      </c>
+      <c r="K12">
+        <f>K7/29.97</f>
+        <v>263.0296963630297</v>
+      </c>
+      <c r="M12">
+        <f>M7/29.97</f>
+        <v>270.17017017017019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <f>K12-J12</f>
+        <v>13.980647313980654</v>
+      </c>
+      <c r="M13">
+        <f>M12-K12</f>
+        <v>7.140473807140495</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <f>J2/29.97</f>
+        <v>294.52786119452787</v>
+      </c>
+      <c r="K14">
+        <f>K2/29.97</f>
+        <v>306.87354020687354</v>
+      </c>
+      <c r="M14">
+        <f>M2/29.97</f>
+        <v>312.84617951284616</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <f>K14-J14</f>
+        <v>12.34567901234567</v>
+      </c>
+      <c r="M15">
+        <f>M14-K14</f>
+        <v>5.9726393059726206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>